<commit_message>
Werkende verzoeken naar de Clash Royale API
</commit_message>
<xml_diff>
--- a/clanoverview_logs/logs/2017-12-21_clanoverzicht.xlsx
+++ b/clanoverview_logs/logs/2017-12-21_clanoverzicht.xlsx
@@ -185,42 +185,42 @@
     <t>member</t>
   </si>
   <si>
+    <t>Ronald O</t>
+  </si>
+  <si>
+    <t>#99UJ999G</t>
+  </si>
+  <si>
+    <t>Shyngalicious</t>
+  </si>
+  <si>
+    <t>#RLCLPJ</t>
+  </si>
+  <si>
+    <t>Wolverine</t>
+  </si>
+  <si>
+    <t>#828YUV9J</t>
+  </si>
+  <si>
+    <t>peter</t>
+  </si>
+  <si>
+    <t>#8LV09JG9</t>
+  </si>
+  <si>
+    <t>elandro</t>
+  </si>
+  <si>
+    <t>#22GU992L</t>
+  </si>
+  <si>
     <t>pamuk39</t>
   </si>
   <si>
     <t>#RV8JG08P</t>
   </si>
   <si>
-    <t>Ronald O</t>
-  </si>
-  <si>
-    <t>#99UJ999G</t>
-  </si>
-  <si>
-    <t>Shyngalicious</t>
-  </si>
-  <si>
-    <t>#RLCLPJ</t>
-  </si>
-  <si>
-    <t>Wolverine</t>
-  </si>
-  <si>
-    <t>#828YUV9J</t>
-  </si>
-  <si>
-    <t>elandro</t>
-  </si>
-  <si>
-    <t>#22GU992L</t>
-  </si>
-  <si>
-    <t>peter</t>
-  </si>
-  <si>
-    <t>#8LV09JG9</t>
-  </si>
-  <si>
     <t>mauzer99</t>
   </si>
   <si>
@@ -275,22 +275,22 @@
     <t>#C0UC2QPJ</t>
   </si>
   <si>
+    <t>OhhJayky!</t>
+  </si>
+  <si>
+    <t>#R0Y2J8G2</t>
+  </si>
+  <si>
+    <t>Lol-with-pohl</t>
+  </si>
+  <si>
+    <t>#G2UGVYCJ</t>
+  </si>
+  <si>
     <t>marco25</t>
   </si>
   <si>
     <t>#9CGP2Y2G</t>
-  </si>
-  <si>
-    <t>OhhJayky!</t>
-  </si>
-  <si>
-    <t>#R0Y2J8G2</t>
-  </si>
-  <si>
-    <t>Lol-with-pohl</t>
-  </si>
-  <si>
-    <t>#G2UGVYCJ</t>
   </si>
   <si>
     <t>Duke en wes</t>
@@ -439,19 +439,19 @@
         <v>211.0</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>5742.0</v>
+        <v>5747.0</v>
       </c>
       <c r="F2" t="s">
         <v>11</v>
       </c>
       <c r="G2" s="2" t="n">
-        <v>5468.0</v>
+        <v>5538.0</v>
       </c>
       <c r="H2" s="2" t="n">
-        <v>5582.0</v>
+        <v>5619.0</v>
       </c>
       <c r="I2" s="2" t="n">
-        <v>0.98</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         <v>197.0</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>5539.0</v>
+        <v>5535.0</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>14</v>
@@ -497,19 +497,19 @@
         <v>179.0</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>5369.0</v>
+        <v>5377.0</v>
       </c>
       <c r="F4" t="s">
         <v>14</v>
       </c>
       <c r="G4" s="2" t="n">
-        <v>1484.0</v>
+        <v>1563.0</v>
       </c>
       <c r="H4" s="2" t="n">
-        <v>1496.0</v>
+        <v>1533.0</v>
       </c>
       <c r="I4" s="2" t="n">
-        <v>0.99</v>
+        <v>1.02</v>
       </c>
     </row>
     <row r="5">
@@ -561,13 +561,13 @@
         <v>21</v>
       </c>
       <c r="G6" s="2" t="n">
-        <v>4164.0</v>
+        <v>4194.0</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>3585.0</v>
       </c>
       <c r="I6" s="2" t="n">
-        <v>1.16</v>
+        <v>1.17</v>
       </c>
     </row>
     <row r="7">
@@ -584,19 +584,19 @@
         <v>184.0</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>5066.0</v>
+        <v>5075.0</v>
       </c>
       <c r="F7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G7" s="3" t="n">
-        <v>1889.0</v>
+        <v>1900.0</v>
       </c>
       <c r="H7" s="3" t="n">
         <v>1423.0</v>
       </c>
       <c r="I7" s="3" t="n">
-        <v>1.33</v>
+        <v>1.34</v>
       </c>
     </row>
     <row r="8">
@@ -642,19 +642,19 @@
         <v>210.0</v>
       </c>
       <c r="E9" s="3" t="n">
-        <v>4933.0</v>
+        <v>4931.0</v>
       </c>
       <c r="F9" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G9" s="3" t="n">
-        <v>5620.0</v>
+        <v>5657.0</v>
       </c>
       <c r="H9" s="3" t="n">
-        <v>2825.0</v>
+        <v>2897.0</v>
       </c>
       <c r="I9" s="3" t="n">
-        <v>1.99</v>
+        <v>1.95</v>
       </c>
     </row>
     <row r="10">
@@ -700,19 +700,19 @@
         <v>172.0</v>
       </c>
       <c r="E11" s="3" t="n">
-        <v>4876.0</v>
+        <v>4907.0</v>
       </c>
       <c r="F11" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G11" s="3" t="n">
-        <v>3013.0</v>
+        <v>3122.0</v>
       </c>
       <c r="H11" s="3" t="n">
-        <v>2678.0</v>
+        <v>2710.0</v>
       </c>
       <c r="I11" s="3" t="n">
-        <v>1.13</v>
+        <v>1.15</v>
       </c>
     </row>
     <row r="12">
@@ -735,13 +735,13 @@
         <v>14</v>
       </c>
       <c r="G12" s="2" t="n">
-        <v>1185.0</v>
+        <v>1187.0</v>
       </c>
       <c r="H12" s="2" t="n">
-        <v>1809.0</v>
+        <v>1844.0</v>
       </c>
       <c r="I12" s="2" t="n">
-        <v>0.66</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="13">
@@ -758,19 +758,19 @@
         <v>174.0</v>
       </c>
       <c r="E13" s="3" t="n">
-        <v>4858.0</v>
+        <v>4864.0</v>
       </c>
       <c r="F13" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G13" s="3" t="n">
-        <v>3876.0</v>
+        <v>3949.0</v>
       </c>
       <c r="H13" s="3" t="n">
-        <v>5948.0</v>
+        <v>5983.0</v>
       </c>
       <c r="I13" s="3" t="n">
-        <v>0.65</v>
+        <v>0.66</v>
       </c>
     </row>
     <row r="14">
@@ -793,13 +793,13 @@
         <v>21</v>
       </c>
       <c r="G14" s="2" t="n">
-        <v>3411.0</v>
+        <v>3441.0</v>
       </c>
       <c r="H14" s="2" t="n">
-        <v>3711.0</v>
+        <v>3785.0</v>
       </c>
       <c r="I14" s="2" t="n">
-        <v>0.92</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="15">
@@ -816,7 +816,7 @@
         <v>175.0</v>
       </c>
       <c r="E15" s="3" t="n">
-        <v>4794.0</v>
+        <v>4827.0</v>
       </c>
       <c r="F15" s="4" t="s">
         <v>14</v>
@@ -825,10 +825,10 @@
         <v>1525.0</v>
       </c>
       <c r="H15" s="3" t="n">
-        <v>2194.0</v>
+        <v>2231.0</v>
       </c>
       <c r="I15" s="3" t="n">
-        <v>0.7</v>
+        <v>0.68</v>
       </c>
     </row>
     <row r="16">
@@ -845,19 +845,19 @@
         <v>178.0</v>
       </c>
       <c r="E16" s="2" t="n">
-        <v>4756.0</v>
+        <v>4759.0</v>
       </c>
       <c r="F16" t="s">
         <v>14</v>
       </c>
       <c r="G16" s="2" t="n">
-        <v>5234.0</v>
+        <v>5403.0</v>
       </c>
       <c r="H16" s="2" t="n">
-        <v>6616.0</v>
+        <v>6760.0</v>
       </c>
       <c r="I16" s="2" t="n">
-        <v>0.79</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="17">
@@ -874,19 +874,19 @@
         <v>179.0</v>
       </c>
       <c r="E17" s="3" t="n">
-        <v>4706.0</v>
+        <v>4729.0</v>
       </c>
       <c r="F17" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G17" s="3" t="n">
-        <v>1456.0</v>
+        <v>1495.0</v>
       </c>
       <c r="H17" s="3" t="n">
-        <v>2149.0</v>
+        <v>2332.0</v>
       </c>
       <c r="I17" s="3" t="n">
-        <v>0.68</v>
+        <v>0.64</v>
       </c>
     </row>
     <row r="18">
@@ -903,19 +903,19 @@
         <v>191.0</v>
       </c>
       <c r="E18" s="2" t="n">
-        <v>4678.0</v>
+        <v>4676.0</v>
       </c>
       <c r="F18" t="s">
         <v>21</v>
       </c>
       <c r="G18" s="2" t="n">
-        <v>1554.0</v>
+        <v>1633.0</v>
       </c>
       <c r="H18" s="2" t="n">
-        <v>1337.0</v>
+        <v>1374.0</v>
       </c>
       <c r="I18" s="2" t="n">
-        <v>1.16</v>
+        <v>1.19</v>
       </c>
     </row>
     <row r="19">
@@ -941,7 +941,7 @@
         <v>7025.0</v>
       </c>
       <c r="H19" s="3" t="n">
-        <v>7149.0</v>
+        <v>7186.0</v>
       </c>
       <c r="I19" s="3" t="n">
         <v>0.98</v>
@@ -961,19 +961,19 @@
         <v>211.0</v>
       </c>
       <c r="E20" s="2" t="n">
-        <v>4637.0</v>
+        <v>4654.0</v>
       </c>
       <c r="F20" t="s">
         <v>14</v>
       </c>
       <c r="G20" s="2" t="n">
-        <v>6894.0</v>
+        <v>6961.0</v>
       </c>
       <c r="H20" s="2" t="n">
-        <v>4336.0</v>
+        <v>4517.0</v>
       </c>
       <c r="I20" s="2" t="n">
-        <v>1.59</v>
+        <v>1.54</v>
       </c>
     </row>
     <row r="21">
@@ -1074,22 +1074,22 @@
         <v>58</v>
       </c>
       <c r="D24" s="2" t="n">
-        <v>195.0</v>
+        <v>163.0</v>
       </c>
       <c r="E24" s="2" t="n">
-        <v>4479.0</v>
+        <v>4465.0</v>
       </c>
       <c r="F24" t="s">
         <v>14</v>
       </c>
       <c r="G24" s="2" t="n">
-        <v>6862.0</v>
+        <v>2577.0</v>
       </c>
       <c r="H24" s="2" t="n">
-        <v>4003.0</v>
+        <v>3386.0</v>
       </c>
       <c r="I24" s="2" t="n">
-        <v>1.71</v>
+        <v>0.76</v>
       </c>
     </row>
     <row r="25">
@@ -1103,22 +1103,22 @@
         <v>60</v>
       </c>
       <c r="D25" s="3" t="n">
-        <v>163.0</v>
+        <v>149.0</v>
       </c>
       <c r="E25" s="3" t="n">
-        <v>4465.0</v>
+        <v>4447.0</v>
       </c>
       <c r="F25" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G25" s="3" t="n">
-        <v>2577.0</v>
+        <v>1296.0</v>
       </c>
       <c r="H25" s="3" t="n">
-        <v>3386.0</v>
+        <v>2247.0</v>
       </c>
       <c r="I25" s="3" t="n">
-        <v>0.76</v>
+        <v>0.58</v>
       </c>
     </row>
     <row r="26">
@@ -1132,22 +1132,22 @@
         <v>62</v>
       </c>
       <c r="D26" s="2" t="n">
-        <v>149.0</v>
+        <v>161.0</v>
       </c>
       <c r="E26" s="2" t="n">
-        <v>4453.0</v>
+        <v>4395.0</v>
       </c>
       <c r="F26" t="s">
-        <v>14</v>
+        <v>56</v>
       </c>
       <c r="G26" s="2" t="n">
-        <v>1296.0</v>
+        <v>1095.0</v>
       </c>
       <c r="H26" s="2" t="n">
-        <v>2247.0</v>
+        <v>1636.0</v>
       </c>
       <c r="I26" s="2" t="n">
-        <v>0.58</v>
+        <v>0.67</v>
       </c>
     </row>
     <row r="27">
@@ -1161,22 +1161,22 @@
         <v>64</v>
       </c>
       <c r="D27" s="3" t="n">
-        <v>161.0</v>
+        <v>159.0</v>
       </c>
       <c r="E27" s="3" t="n">
-        <v>4388.0</v>
+        <v>4323.0</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>56</v>
+        <v>14</v>
       </c>
       <c r="G27" s="3" t="n">
-        <v>1095.0</v>
+        <v>2384.0</v>
       </c>
       <c r="H27" s="3" t="n">
-        <v>1599.0</v>
+        <v>3405.0</v>
       </c>
       <c r="I27" s="3" t="n">
-        <v>0.68</v>
+        <v>0.7</v>
       </c>
     </row>
     <row r="28">
@@ -1199,13 +1199,13 @@
         <v>14</v>
       </c>
       <c r="G28" s="2" t="n">
-        <v>3257.0</v>
+        <v>3437.0</v>
       </c>
       <c r="H28" s="2" t="n">
         <v>4071.0</v>
       </c>
       <c r="I28" s="2" t="n">
-        <v>0.8</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="29">
@@ -1219,22 +1219,22 @@
         <v>68</v>
       </c>
       <c r="D29" s="3" t="n">
-        <v>159.0</v>
+        <v>195.0</v>
       </c>
       <c r="E29" s="3" t="n">
-        <v>4295.0</v>
+        <v>4278.0</v>
       </c>
       <c r="F29" s="4" t="s">
         <v>14</v>
       </c>
       <c r="G29" s="3" t="n">
-        <v>2275.0</v>
+        <v>7017.0</v>
       </c>
       <c r="H29" s="3" t="n">
-        <v>3331.0</v>
+        <v>4373.0</v>
       </c>
       <c r="I29" s="3" t="n">
-        <v>0.68</v>
+        <v>1.6</v>
       </c>
     </row>
     <row r="30">
@@ -1260,10 +1260,10 @@
         <v>68.0</v>
       </c>
       <c r="H30" s="2" t="n">
-        <v>183.0</v>
+        <v>218.0</v>
       </c>
       <c r="I30" s="2" t="n">
-        <v>0.37</v>
+        <v>0.31</v>
       </c>
     </row>
     <row r="31">
@@ -1309,7 +1309,7 @@
         <v>168.0</v>
       </c>
       <c r="E32" s="2" t="n">
-        <v>3944.0</v>
+        <v>3942.0</v>
       </c>
       <c r="F32" t="s">
         <v>21</v>
@@ -1338,7 +1338,7 @@
         <v>155.0</v>
       </c>
       <c r="E33" s="3" t="n">
-        <v>3760.0</v>
+        <v>3771.0</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>21</v>
@@ -1347,10 +1347,10 @@
         <v>1682.0</v>
       </c>
       <c r="H33" s="3" t="n">
-        <v>1680.0</v>
+        <v>1751.0</v>
       </c>
       <c r="I33" s="3" t="n">
-        <v>1.0</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="34">
@@ -1367,19 +1367,19 @@
         <v>170.0</v>
       </c>
       <c r="E34" s="2" t="n">
-        <v>3675.0</v>
+        <v>3713.0</v>
       </c>
       <c r="F34" t="s">
         <v>14</v>
       </c>
       <c r="G34" s="2" t="n">
-        <v>7651.0</v>
+        <v>7790.0</v>
       </c>
       <c r="H34" s="2" t="n">
-        <v>5803.0</v>
+        <v>5951.0</v>
       </c>
       <c r="I34" s="2" t="n">
-        <v>1.32</v>
+        <v>1.31</v>
       </c>
     </row>
     <row r="35">
@@ -1425,7 +1425,7 @@
         <v>131.0</v>
       </c>
       <c r="E36" s="2" t="n">
-        <v>3508.0</v>
+        <v>3492.0</v>
       </c>
       <c r="F36" t="s">
         <v>56</v>
@@ -1454,7 +1454,7 @@
         <v>156.0</v>
       </c>
       <c r="E37" s="3" t="n">
-        <v>3498.0</v>
+        <v>3429.0</v>
       </c>
       <c r="F37" s="4" t="s">
         <v>56</v>
@@ -1463,10 +1463,10 @@
         <v>853.0</v>
       </c>
       <c r="H37" s="3" t="n">
-        <v>676.0</v>
+        <v>713.0</v>
       </c>
       <c r="I37" s="3" t="n">
-        <v>1.26</v>
+        <v>1.2</v>
       </c>
     </row>
     <row r="38">
@@ -1483,7 +1483,7 @@
         <v>151.0</v>
       </c>
       <c r="E38" s="2" t="n">
-        <v>3417.0</v>
+        <v>3407.0</v>
       </c>
       <c r="F38" t="s">
         <v>14</v>
@@ -1509,22 +1509,22 @@
         <v>88</v>
       </c>
       <c r="D39" s="3" t="n">
-        <v>214.0</v>
+        <v>123.0</v>
       </c>
       <c r="E39" s="3" t="n">
-        <v>3394.0</v>
+        <v>3296.0</v>
       </c>
       <c r="F39" s="4" t="s">
         <v>21</v>
       </c>
       <c r="G39" s="3" t="n">
-        <v>3663.0</v>
+        <v>639.0</v>
       </c>
       <c r="H39" s="3" t="n">
-        <v>3971.0</v>
+        <v>1062.0</v>
       </c>
       <c r="I39" s="3" t="n">
-        <v>0.92</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="40">
@@ -1538,22 +1538,22 @@
         <v>90</v>
       </c>
       <c r="D40" s="2" t="n">
-        <v>123.0</v>
+        <v>165.0</v>
       </c>
       <c r="E40" s="2" t="n">
-        <v>3296.0</v>
+        <v>3269.0</v>
       </c>
       <c r="F40" t="s">
-        <v>21</v>
+        <v>56</v>
       </c>
       <c r="G40" s="2" t="n">
-        <v>639.0</v>
+        <v>0.0</v>
       </c>
       <c r="H40" s="2" t="n">
-        <v>1062.0</v>
+        <v>0.0</v>
       </c>
       <c r="I40" s="2" t="n">
-        <v>0.6</v>
+        <v>0.0</v>
       </c>
     </row>
     <row r="41">
@@ -1567,22 +1567,22 @@
         <v>92</v>
       </c>
       <c r="D41" s="3" t="n">
-        <v>165.0</v>
+        <v>214.0</v>
       </c>
       <c r="E41" s="3" t="n">
-        <v>3161.0</v>
+        <v>3180.0</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>56</v>
+        <v>21</v>
       </c>
       <c r="G41" s="3" t="n">
-        <v>1417.0</v>
+        <v>4088.0</v>
       </c>
       <c r="H41" s="3" t="n">
-        <v>988.0</v>
+        <v>4119.0</v>
       </c>
       <c r="I41" s="3" t="n">
-        <v>1.43</v>
+        <v>0.99</v>
       </c>
     </row>
     <row r="42">
@@ -1599,19 +1599,19 @@
         <v>112.0</v>
       </c>
       <c r="E42" s="2" t="n">
-        <v>2471.0</v>
+        <v>2494.0</v>
       </c>
       <c r="F42" t="s">
         <v>14</v>
       </c>
       <c r="G42" s="2" t="n">
-        <v>37.0</v>
+        <v>42.0</v>
       </c>
       <c r="H42" s="2" t="n">
         <v>731.0</v>
       </c>
       <c r="I42" s="2" t="n">
-        <v>0.05</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="43">
@@ -1646,7 +1646,7 @@
   </sheetData>
   <pageMargins bottom="0.5" footer="0.3" header="0.3" left="0.25" right="0.25" top="0.5"/>
   <headerFooter>
-    <oddFooter>&amp;LClanoverzicht&amp;R21/12/2017 15:09</oddFooter>
+    <oddFooter>&amp;LClanoverzicht&amp;R21/12/2017 21:55</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>